<commit_message>
add week8 and week9 timesheet t
</commit_message>
<xml_diff>
--- a/Timesheet_a1751414_Jialun Han.xlsx
+++ b/Timesheet_a1751414_Jialun Han.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicahan/Documents/MyUni/MCI/code/Team27/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931E4C80-2C6D-C441-B252-ADFC23126D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D08F30-E720-6B44-A03E-ADE5B233DC15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week3" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,9 @@
     <sheet name="Week6" sheetId="4" r:id="rId4"/>
     <sheet name="MidBreak" sheetId="6" r:id="rId5"/>
     <sheet name="Week7" sheetId="5" r:id="rId6"/>
-    <sheet name="template" sheetId="7" r:id="rId7"/>
+    <sheet name="week8" sheetId="8" r:id="rId7"/>
+    <sheet name="week9" sheetId="9" r:id="rId8"/>
+    <sheet name="template" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Week3!$A$1:$H$17</definedName>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="83">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -274,6 +276,24 @@
   </si>
   <si>
     <t>Look into parsons puzzle js on github</t>
+  </si>
+  <si>
+    <t>Connect js-parson with H5P</t>
+  </si>
+  <si>
+    <t>Draw datagrams of js-parson</t>
+  </si>
+  <si>
+    <t>Paper research</t>
+  </si>
+  <si>
+    <t>Design the system and create a document about design</t>
+  </si>
+  <si>
+    <t>Literature Review of Parsons Puzzle</t>
+  </si>
+  <si>
+    <t>Work on the connection between H5P and Drupal</t>
   </si>
 </sst>
 </file>
@@ -572,7 +592,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -656,6 +676,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1069,16 +1095,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1193,10 +1219,10 @@
       <c r="AT6" s="3"/>
     </row>
     <row r="7" spans="1:46" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="37">
         <v>43907</v>
       </c>
       <c r="C7" s="6">
@@ -1255,8 +1281,8 @@
       <c r="AT7" s="3"/>
     </row>
     <row r="8" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
-      <c r="B8" s="36"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="6">
         <v>0.60416666666666663</v>
       </c>
@@ -1315,8 +1341,8 @@
       <c r="AT8" s="3"/>
     </row>
     <row r="9" spans="1:46" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
-      <c r="B9" s="37"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="6">
         <v>0.63541666666666663</v>
       </c>
@@ -1437,10 +1463,10 @@
       <c r="AT10" s="3"/>
     </row>
     <row r="11" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="37">
         <v>43909</v>
       </c>
       <c r="C11" s="6">
@@ -1499,8 +1525,8 @@
       <c r="AT11" s="3"/>
     </row>
     <row r="12" spans="1:46" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
-      <c r="B12" s="37"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="6">
         <v>0.52083333333333337</v>
       </c>
@@ -1797,16 +1823,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2107,10 +2133,10 @@
       <c r="AT9" s="3"/>
     </row>
     <row r="10" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="37">
         <v>43917</v>
       </c>
       <c r="C10" s="5">
@@ -2169,8 +2195,8 @@
       <c r="AT10" s="3"/>
     </row>
     <row r="11" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="39"/>
-      <c r="B11" s="37"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="5">
         <v>0.375</v>
       </c>
@@ -2407,16 +2433,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2521,10 +2547,10 @@
       <c r="AT6" s="3"/>
     </row>
     <row r="7" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="37">
         <v>43921</v>
       </c>
       <c r="C7" s="6">
@@ -2583,8 +2609,8 @@
       <c r="AT7" s="3"/>
     </row>
     <row r="8" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
-      <c r="B8" s="37"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="6">
         <v>0.60416666666666663</v>
       </c>
@@ -2765,10 +2791,10 @@
       <c r="AT10" s="3"/>
     </row>
     <row r="11" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="37">
         <v>43924</v>
       </c>
       <c r="C11" s="5">
@@ -2827,8 +2853,8 @@
       <c r="AT11" s="3"/>
     </row>
     <row r="12" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="39"/>
-      <c r="B12" s="37"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="5">
         <v>0.58333333333333337</v>
       </c>
@@ -2947,10 +2973,10 @@
       <c r="AT13" s="3"/>
     </row>
     <row r="14" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="40">
+      <c r="B14" s="42">
         <v>43926</v>
       </c>
       <c r="C14" s="6">
@@ -3011,8 +3037,8 @@
       <c r="AT14" s="3"/>
     </row>
     <row r="15" spans="1:46" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="41"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="6">
         <v>0.41666666666666669</v>
       </c>
@@ -3128,16 +3154,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3190,10 +3216,10 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="46">
         <v>43927</v>
       </c>
       <c r="C6" s="5">
@@ -3250,8 +3276,8 @@
       <c r="AT6" s="3"/>
     </row>
     <row r="7" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="43"/>
-      <c r="B7" s="45"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="5">
         <v>0.58333333333333337</v>
       </c>
@@ -3306,10 +3332,10 @@
       <c r="AT7" s="3"/>
     </row>
     <row r="8" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="46">
         <v>43928</v>
       </c>
       <c r="C8" s="6">
@@ -3368,8 +3394,8 @@
       <c r="AT8" s="3"/>
     </row>
     <row r="9" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
-      <c r="B9" s="45"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="6">
         <v>0.64583333333333337</v>
       </c>
@@ -3425,10 +3451,10 @@
       <c r="AT9" s="3"/>
     </row>
     <row r="10" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="46">
         <v>43929</v>
       </c>
       <c r="C10" s="5">
@@ -3487,8 +3513,8 @@
       <c r="AT10" s="3"/>
     </row>
     <row r="11" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="43"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="5">
         <v>0.47916666666666669</v>
       </c>
@@ -3605,10 +3631,10 @@
       <c r="AT12" s="3"/>
     </row>
     <row r="13" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="35">
+      <c r="B13" s="37">
         <v>43931</v>
       </c>
       <c r="C13" s="5">
@@ -3665,8 +3691,8 @@
       <c r="AT13" s="3"/>
     </row>
     <row r="14" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="39"/>
-      <c r="B14" s="37"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="5">
         <v>0.58333333333333337</v>
       </c>
@@ -3886,7 +3912,7 @@
   <dimension ref="A2:AT25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3902,22 +3928,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="30">
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5085,8 +5111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CEDF29-3264-0B4F-93AF-E5B1D2A6DEFD}">
   <dimension ref="A2:AT16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5102,22 +5128,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="30">
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5785,11 +5811,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6D53E5-41C4-1E42-A50A-F4E63F1C68BE}">
-  <dimension ref="A2:AT13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A00F32-F082-3D44-98BF-0BB8F2434DE2}">
+  <dimension ref="A2:AT15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C8" sqref="C8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5805,22 +5831,1300 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="30">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="24">
+        <v>43955</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+    </row>
+    <row r="7" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+    </row>
+    <row r="8" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="32"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AS8" s="3"/>
+      <c r="AT8" s="3"/>
+    </row>
+    <row r="9" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="24">
+        <v>43956</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="7">
+        <v>3</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="3"/>
+      <c r="AT9" s="3"/>
+    </row>
+    <row r="10" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="24">
+        <v>43957</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="E10" s="7">
+        <v>4</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+      <c r="AT10" s="3"/>
+    </row>
+    <row r="11" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="24">
+        <v>43958</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="E11" s="7">
+        <v>4</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="3"/>
+      <c r="AO11" s="3"/>
+      <c r="AP11" s="3"/>
+      <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
+      <c r="AS11" s="3"/>
+      <c r="AT11" s="3"/>
+    </row>
+    <row r="12" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="24">
+        <v>43959</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+      <c r="AT12" s="3"/>
+    </row>
+    <row r="13" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="24">
+        <v>43960</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="E13" s="7">
+        <v>4</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="3"/>
+      <c r="AN13" s="3"/>
+      <c r="AO13" s="3"/>
+      <c r="AP13" s="3"/>
+      <c r="AQ13" s="3"/>
+      <c r="AR13" s="3"/>
+      <c r="AS13" s="3"/>
+      <c r="AT13" s="3"/>
+    </row>
+    <row r="14" spans="1:46" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="24">
+        <v>43961</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="3"/>
+      <c r="AN14" s="3"/>
+      <c r="AO14" s="3"/>
+      <c r="AP14" s="3"/>
+      <c r="AQ14" s="3"/>
+      <c r="AR14" s="3"/>
+      <c r="AS14" s="3"/>
+      <c r="AT14" s="3"/>
+    </row>
+    <row r="15" spans="1:46" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="15">
+        <f>SUM(E6:E14)</f>
+        <v>26</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D14" xr:uid="{133D1DA1-812D-054B-B89D-A7BA999ACFBB}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F05BAE-BECB-1B47-9C1B-175469369053}">
+  <dimension ref="A2:AT15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="18" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" customWidth="1"/>
+    <col min="13" max="46" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="24">
+        <v>43962</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+    </row>
+    <row r="7" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="24">
+        <v>43963</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+    </row>
+    <row r="8" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="31"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AS8" s="3"/>
+      <c r="AT8" s="3"/>
+    </row>
+    <row r="9" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="31"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="3"/>
+      <c r="AT9" s="3"/>
+    </row>
+    <row r="10" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="24">
+        <v>43964</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="E10" s="7">
+        <v>4</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+      <c r="AT10" s="3"/>
+    </row>
+    <row r="11" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="24">
+        <v>43965</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="3"/>
+      <c r="AO11" s="3"/>
+      <c r="AP11" s="3"/>
+      <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
+      <c r="AS11" s="3"/>
+      <c r="AT11" s="3"/>
+    </row>
+    <row r="12" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="24">
+        <v>43966</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="E12" s="7">
+        <v>4</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+      <c r="AT12" s="3"/>
+    </row>
+    <row r="13" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="24">
+        <v>43967</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="7">
+        <v>3</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="3"/>
+      <c r="AN13" s="3"/>
+      <c r="AO13" s="3"/>
+      <c r="AP13" s="3"/>
+      <c r="AQ13" s="3"/>
+      <c r="AR13" s="3"/>
+      <c r="AS13" s="3"/>
+      <c r="AT13" s="3"/>
+    </row>
+    <row r="14" spans="1:46" s="4" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="24">
+        <v>43968</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="3"/>
+      <c r="AN14" s="3"/>
+      <c r="AO14" s="3"/>
+      <c r="AP14" s="3"/>
+      <c r="AQ14" s="3"/>
+      <c r="AR14" s="3"/>
+      <c r="AS14" s="3"/>
+      <c r="AT14" s="3"/>
+    </row>
+    <row r="15" spans="1:46" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="15">
+        <f>SUM(E6:E14)</f>
+        <v>24</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D14" xr:uid="{626B47F3-B8A9-184B-B7EE-CDB0B4DBF556}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6D53E5-41C4-1E42-A50A-F4E63F1C68BE}">
+  <dimension ref="A2:AT13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="18" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" customWidth="1"/>
+    <col min="13" max="46" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30">
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">

</xml_diff>

<commit_message>
test function of branch
</commit_message>
<xml_diff>
--- a/Timesheet_a1751414_Jialun Han.xlsx
+++ b/Timesheet_a1751414_Jialun Han.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicahan/Documents/MyUni/MCI/code/Team27/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D08F30-E720-6B44-A03E-ADE5B233DC15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883B2EDC-521C-324C-A6E8-1CDBA74E061B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week3" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="Week7" sheetId="5" r:id="rId6"/>
     <sheet name="week8" sheetId="8" r:id="rId7"/>
     <sheet name="week9" sheetId="9" r:id="rId8"/>
-    <sheet name="template" sheetId="7" r:id="rId9"/>
+    <sheet name="week10" sheetId="10" r:id="rId9"/>
+    <sheet name="template" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Week3!$A$1:$H$17</definedName>
@@ -1802,6 +1803,485 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6D53E5-41C4-1E42-A50A-F4E63F1C68BE}">
+  <dimension ref="A2:AT13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="18" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" customWidth="1"/>
+    <col min="13" max="46" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="24">
+        <v>43934</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+    </row>
+    <row r="7" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="24">
+        <v>43935</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+    </row>
+    <row r="8" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="24">
+        <v>43936</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AS8" s="3"/>
+      <c r="AT8" s="3"/>
+    </row>
+    <row r="9" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="24">
+        <v>43937</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="3"/>
+      <c r="AT9" s="3"/>
+    </row>
+    <row r="10" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="26">
+        <v>43938</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+      <c r="AT10" s="3"/>
+    </row>
+    <row r="11" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="24">
+        <v>43939</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="3"/>
+      <c r="AO11" s="3"/>
+      <c r="AP11" s="3"/>
+      <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
+      <c r="AS11" s="3"/>
+      <c r="AT11" s="3"/>
+    </row>
+    <row r="12" spans="1:46" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="24">
+        <v>43940</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+      <c r="AT12" s="3"/>
+    </row>
+    <row r="13" spans="1:46" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="15">
+        <f>SUM(E6:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D12" xr:uid="{A701FE38-3227-AE40-88C3-1821690D15E4}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07650CC-4E9E-DF40-8F16-16A37E275F26}">
   <dimension ref="A2:AT14"/>
@@ -6453,7 +6933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F05BAE-BECB-1B47-9C1B-175469369053}">
   <dimension ref="A2:AT15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -7089,480 +7569,13 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6D53E5-41C4-1E42-A50A-F4E63F1C68BE}">
-  <dimension ref="A2:AT13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F2A0E12-6403-8F47-9944-0498485D6D04}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="18" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.6640625" customWidth="1"/>
-    <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" customWidth="1"/>
-    <col min="13" max="46" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-    </row>
-    <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="30">
-        <v>27</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:46" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="24">
-        <v>43934</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
-      <c r="AJ6" s="3"/>
-      <c r="AK6" s="3"/>
-      <c r="AL6" s="3"/>
-      <c r="AM6" s="3"/>
-      <c r="AN6" s="3"/>
-      <c r="AO6" s="3"/>
-      <c r="AP6" s="3"/>
-      <c r="AQ6" s="3"/>
-      <c r="AR6" s="3"/>
-      <c r="AS6" s="3"/>
-      <c r="AT6" s="3"/>
-    </row>
-    <row r="7" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="24">
-        <v>43935</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="3"/>
-      <c r="AJ7" s="3"/>
-      <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="3"/>
-      <c r="AO7" s="3"/>
-      <c r="AP7" s="3"/>
-      <c r="AQ7" s="3"/>
-      <c r="AR7" s="3"/>
-      <c r="AS7" s="3"/>
-      <c r="AT7" s="3"/>
-    </row>
-    <row r="8" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="24">
-        <v>43936</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
-      <c r="AJ8" s="3"/>
-      <c r="AK8" s="3"/>
-      <c r="AL8" s="3"/>
-      <c r="AM8" s="3"/>
-      <c r="AN8" s="3"/>
-      <c r="AO8" s="3"/>
-      <c r="AP8" s="3"/>
-      <c r="AQ8" s="3"/>
-      <c r="AR8" s="3"/>
-      <c r="AS8" s="3"/>
-      <c r="AT8" s="3"/>
-    </row>
-    <row r="9" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="24">
-        <v>43937</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
-      <c r="AJ9" s="3"/>
-      <c r="AK9" s="3"/>
-      <c r="AL9" s="3"/>
-      <c r="AM9" s="3"/>
-      <c r="AN9" s="3"/>
-      <c r="AO9" s="3"/>
-      <c r="AP9" s="3"/>
-      <c r="AQ9" s="3"/>
-      <c r="AR9" s="3"/>
-      <c r="AS9" s="3"/>
-      <c r="AT9" s="3"/>
-    </row>
-    <row r="10" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="26">
-        <v>43938</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
-      <c r="AJ10" s="3"/>
-      <c r="AK10" s="3"/>
-      <c r="AL10" s="3"/>
-      <c r="AM10" s="3"/>
-      <c r="AN10" s="3"/>
-      <c r="AO10" s="3"/>
-      <c r="AP10" s="3"/>
-      <c r="AQ10" s="3"/>
-      <c r="AR10" s="3"/>
-      <c r="AS10" s="3"/>
-      <c r="AT10" s="3"/>
-    </row>
-    <row r="11" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="24">
-        <v>43939</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="3"/>
-      <c r="AJ11" s="3"/>
-      <c r="AK11" s="3"/>
-      <c r="AL11" s="3"/>
-      <c r="AM11" s="3"/>
-      <c r="AN11" s="3"/>
-      <c r="AO11" s="3"/>
-      <c r="AP11" s="3"/>
-      <c r="AQ11" s="3"/>
-      <c r="AR11" s="3"/>
-      <c r="AS11" s="3"/>
-      <c r="AT11" s="3"/>
-    </row>
-    <row r="12" spans="1:46" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="24">
-        <v>43940</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="3"/>
-      <c r="AB12" s="3"/>
-      <c r="AC12" s="3"/>
-      <c r="AD12" s="3"/>
-      <c r="AE12" s="3"/>
-      <c r="AF12" s="3"/>
-      <c r="AG12" s="3"/>
-      <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
-      <c r="AJ12" s="3"/>
-      <c r="AK12" s="3"/>
-      <c r="AL12" s="3"/>
-      <c r="AM12" s="3"/>
-      <c r="AN12" s="3"/>
-      <c r="AO12" s="3"/>
-      <c r="AP12" s="3"/>
-      <c r="AQ12" s="3"/>
-      <c r="AR12" s="3"/>
-      <c r="AS12" s="3"/>
-      <c r="AT12" s="3"/>
-    </row>
-    <row r="13" spans="1:46" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="15">
-        <f>SUM(E6:E12)</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:H2"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D12" xr:uid="{A701FE38-3227-AE40-88C3-1821690D15E4}">
-      <formula1>0</formula1>
-      <formula2>0.999305555555556</formula2>
-    </dataValidation>
-  </dataValidations>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update timesheet to week12
</commit_message>
<xml_diff>
--- a/Timesheet_a1751414_Jialun Han.xlsx
+++ b/Timesheet_a1751414_Jialun Han.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicahan/Documents/MyUni/MCI/code/Team27/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197DA15E-6EA4-3B44-942D-8EC1ADCE03CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAFD552-2C83-BD48-9A74-EC70038FE33D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week3" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <sheet name="week8" sheetId="8" r:id="rId7"/>
     <sheet name="week9" sheetId="9" r:id="rId8"/>
     <sheet name="week10" sheetId="10" r:id="rId9"/>
-    <sheet name="template" sheetId="7" r:id="rId10"/>
+    <sheet name="week11" sheetId="11" r:id="rId10"/>
+    <sheet name="week12" sheetId="12" r:id="rId11"/>
+    <sheet name="template" sheetId="7" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Week3!$A$1:$H$17</definedName>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="93">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -307,6 +309,24 @@
   </si>
   <si>
     <t>Work on the fill in the blank function</t>
+  </si>
+  <si>
+    <t>Debug fill in the blank function</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>debug fill in the blank function</t>
+  </si>
+  <si>
+    <t>Contruct system architecture and key components of the Poster</t>
+  </si>
+  <si>
+    <t>Fix code bugs for UI</t>
+  </si>
+  <si>
+    <t>Debug fill in the blank</t>
   </si>
 </sst>
 </file>
@@ -606,7 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -690,6 +710,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1098,7 +1124,7 @@
   </sheetPr>
   <dimension ref="A2:AT16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1115,16 +1141,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1239,10 +1265,10 @@
       <c r="AT6" s="3"/>
     </row>
     <row r="7" spans="1:46" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="41">
         <v>43907</v>
       </c>
       <c r="C7" s="6">
@@ -1301,8 +1327,8 @@
       <c r="AT7" s="3"/>
     </row>
     <row r="8" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="40"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="6">
         <v>0.60416666666666663</v>
       </c>
@@ -1361,8 +1387,8 @@
       <c r="AT8" s="3"/>
     </row>
     <row r="9" spans="1:46" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="38"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="6">
         <v>0.63541666666666663</v>
       </c>
@@ -1483,10 +1509,10 @@
       <c r="AT10" s="3"/>
     </row>
     <row r="11" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="41">
         <v>43909</v>
       </c>
       <c r="C11" s="6">
@@ -1545,8 +1571,8 @@
       <c r="AT11" s="3"/>
     </row>
     <row r="12" spans="1:46" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="6">
         <v>0.52083333333333337</v>
       </c>
@@ -1823,11 +1849,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6D53E5-41C4-1E42-A50A-F4E63F1C68BE}">
-  <dimension ref="A2:AT13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0310FC0-D52B-D64E-81C3-7A6069283E54}">
+  <dimension ref="A2:AT15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1843,16 +1869,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1871,7 +1897,7 @@
         <v>34</v>
       </c>
       <c r="H3">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:46" ht="17" x14ac:dyDescent="0.2">
@@ -1909,7 +1935,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="24">
-        <v>43934</v>
+        <v>43976</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1956,12 +1982,633 @@
       <c r="AS6" s="3"/>
       <c r="AT6" s="3"/>
     </row>
+    <row r="7" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="24">
+        <v>43977</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="E7" s="7">
+        <v>12</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+    </row>
+    <row r="8" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="24">
+        <v>43978</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E8" s="7">
+        <v>10</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AS8" s="3"/>
+      <c r="AT8" s="3"/>
+    </row>
+    <row r="9" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="24">
+        <v>43979</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="3"/>
+      <c r="AT9" s="3"/>
+    </row>
+    <row r="10" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="35"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+      <c r="AT10" s="3"/>
+    </row>
+    <row r="11" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="35"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="3"/>
+      <c r="AO11" s="3"/>
+      <c r="AP11" s="3"/>
+      <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
+      <c r="AS11" s="3"/>
+      <c r="AT11" s="3"/>
+    </row>
+    <row r="12" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="24">
+        <v>43980</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+      <c r="AT12" s="3"/>
+    </row>
+    <row r="13" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="24">
+        <v>43981</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="3"/>
+      <c r="AN13" s="3"/>
+      <c r="AO13" s="3"/>
+      <c r="AP13" s="3"/>
+      <c r="AQ13" s="3"/>
+      <c r="AR13" s="3"/>
+      <c r="AS13" s="3"/>
+      <c r="AT13" s="3"/>
+    </row>
+    <row r="14" spans="1:46" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="24">
+        <v>43982</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="3"/>
+      <c r="AN14" s="3"/>
+      <c r="AO14" s="3"/>
+      <c r="AP14" s="3"/>
+      <c r="AQ14" s="3"/>
+      <c r="AR14" s="3"/>
+      <c r="AS14" s="3"/>
+      <c r="AT14" s="3"/>
+    </row>
+    <row r="15" spans="1:46" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="15">
+        <f>SUM(E6:E14)</f>
+        <v>27.5</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D14" xr:uid="{E94530DE-9B9A-A042-8534-1DEA736889C4}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B676ADA4-5E24-D045-8E39-2BA081963C70}">
+  <dimension ref="A2:AT13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="18" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" customWidth="1"/>
+    <col min="13" max="46" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+    </row>
+    <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="24">
+        <v>43983</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+    </row>
     <row r="7" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="35" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="24">
-        <v>43935</v>
+        <v>43984</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -2008,6 +2655,517 @@
       <c r="AS7" s="3"/>
       <c r="AT7" s="3"/>
     </row>
+    <row r="8" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="24">
+        <v>43985</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="E8" s="7">
+        <v>8</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AS8" s="3"/>
+      <c r="AT8" s="3"/>
+    </row>
+    <row r="9" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="24">
+        <v>43986</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="3"/>
+      <c r="AT9" s="3"/>
+    </row>
+    <row r="10" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="24">
+        <v>43987</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+      <c r="AT10" s="3"/>
+    </row>
+    <row r="11" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="24">
+        <v>43988</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="E11" s="7">
+        <v>8</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="3"/>
+      <c r="AO11" s="3"/>
+      <c r="AP11" s="3"/>
+      <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
+      <c r="AS11" s="3"/>
+      <c r="AT11" s="3"/>
+    </row>
+    <row r="12" spans="1:46" s="4" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="24">
+        <v>43989</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E12" s="7">
+        <v>13</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+      <c r="AT12" s="3"/>
+    </row>
+    <row r="13" spans="1:46" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="15">
+        <f>SUM(E6:E12)</f>
+        <v>29.5</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D12" xr:uid="{1DC5C650-9D6D-7648-BBBC-19A217D58B24}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6D53E5-41C4-1E42-A50A-F4E63F1C68BE}">
+  <dimension ref="A2:AT13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="18" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" customWidth="1"/>
+    <col min="13" max="46" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+    </row>
+    <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="24">
+        <v>43934</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+    </row>
+    <row r="7" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="24">
+        <v>43935</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+    </row>
     <row r="8" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>13</v>
@@ -2322,16 +3480,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2632,10 +3790,10 @@
       <c r="AT9" s="3"/>
     </row>
     <row r="10" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="41">
         <v>43917</v>
       </c>
       <c r="C10" s="5">
@@ -2694,8 +3852,8 @@
       <c r="AT10" s="3"/>
     </row>
     <row r="11" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="43"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="5">
         <v>0.375</v>
       </c>
@@ -2932,16 +4090,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3046,10 +4204,10 @@
       <c r="AT6" s="3"/>
     </row>
     <row r="7" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="41">
         <v>43921</v>
       </c>
       <c r="C7" s="6">
@@ -3108,8 +4266,8 @@
       <c r="AT7" s="3"/>
     </row>
     <row r="8" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="38"/>
-      <c r="B8" s="41"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="6">
         <v>0.60416666666666663</v>
       </c>
@@ -3290,10 +4448,10 @@
       <c r="AT10" s="3"/>
     </row>
     <row r="11" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="41">
         <v>43924</v>
       </c>
       <c r="C11" s="5">
@@ -3352,8 +4510,8 @@
       <c r="AT11" s="3"/>
     </row>
     <row r="12" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="43"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="5">
         <v>0.58333333333333337</v>
       </c>
@@ -3472,10 +4630,10 @@
       <c r="AT13" s="3"/>
     </row>
     <row r="14" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="46">
         <v>43926</v>
       </c>
       <c r="C14" s="6">
@@ -3536,8 +4694,8 @@
       <c r="AT14" s="3"/>
     </row>
     <row r="15" spans="1:46" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
-      <c r="B15" s="45"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="6">
         <v>0.41666666666666669</v>
       </c>
@@ -3653,16 +4811,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3715,10 +4873,10 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="50">
         <v>43927</v>
       </c>
       <c r="C6" s="5">
@@ -3775,8 +4933,8 @@
       <c r="AT6" s="3"/>
     </row>
     <row r="7" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
-      <c r="B7" s="49"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="5">
         <v>0.58333333333333337</v>
       </c>
@@ -3831,10 +4989,10 @@
       <c r="AT7" s="3"/>
     </row>
     <row r="8" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="50">
         <v>43928</v>
       </c>
       <c r="C8" s="6">
@@ -3893,8 +5051,8 @@
       <c r="AT8" s="3"/>
     </row>
     <row r="9" spans="1:46" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="51"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="6">
         <v>0.64583333333333337</v>
       </c>
@@ -3950,10 +5108,10 @@
       <c r="AT9" s="3"/>
     </row>
     <row r="10" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="48">
+      <c r="B10" s="50">
         <v>43929</v>
       </c>
       <c r="C10" s="5">
@@ -4012,8 +5170,8 @@
       <c r="AT10" s="3"/>
     </row>
     <row r="11" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="47"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="5">
         <v>0.47916666666666669</v>
       </c>
@@ -4130,10 +5288,10 @@
       <c r="AT12" s="3"/>
     </row>
     <row r="13" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="39">
+      <c r="B13" s="41">
         <v>43931</v>
       </c>
       <c r="C13" s="5">
@@ -4190,8 +5348,8 @@
       <c r="AT13" s="3"/>
     </row>
     <row r="14" spans="1:46" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="43"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="5">
         <v>0.58333333333333337</v>
       </c>
@@ -4427,16 +5585,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -5627,16 +6785,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -6330,16 +7488,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -6969,16 +8127,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -7591,7 +8749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F2A0E12-6403-8F47-9944-0498485D6D04}">
   <dimension ref="A2:AT13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -7608,16 +8766,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">

</xml_diff>